<commit_message>
added version 1 speach and pres
</commit_message>
<xml_diff>
--- a/ВКР/Презентация/Примеры.xlsx
+++ b/ВКР/Презентация/Примеры.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Учёба\8 Семестр\ВКР\Презентация\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E5CC11-234E-421D-8D54-D2EFD2CEA345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE92AA14-BCC7-4B64-AC50-D65A4FEC5C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>Время транзакции</t>
   </si>
   <si>
     <t>Команда</t>
+  </si>
+  <si>
+    <t>Последовательность</t>
+  </si>
+  <si>
+    <t>Поддержка</t>
+  </si>
+  <si>
+    <t>&lt;1, 2&gt;</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>Сессия 1:</t>
+  </si>
+  <si>
+    <t>Сессия 2:</t>
+  </si>
+  <si>
+    <t>Сессия 3:</t>
+  </si>
+  <si>
+    <t>Сессия 4:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,8 +76,15 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -63,6 +94,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -94,12 +131,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -382,96 +444,365 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="3"/>
+    <col min="13" max="13" width="25.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="33" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="10"/>
+      <c r="M1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12">
+        <v>7</v>
+      </c>
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>8</v>
+      </c>
+      <c r="J4" s="12">
+        <v>8</v>
+      </c>
+      <c r="K4" s="12">
+        <v>2</v>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E5" s="5"/>
+      <c r="J5" s="13">
+        <v>9</v>
+      </c>
+      <c r="K5" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="33" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E6" s="5"/>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="G7" s="2">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>8</v>
+      </c>
+      <c r="J8" s="13">
+        <v>7</v>
+      </c>
+      <c r="K8" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>8</v>
+      </c>
+      <c r="J9" s="12">
+        <v>8</v>
+      </c>
+      <c r="K9" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J10" s="12">
+        <v>9</v>
+      </c>
+      <c r="K10" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="33" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="G13" s="2">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>8</v>
+      </c>
+      <c r="J13" s="12">
+        <v>7</v>
+      </c>
+      <c r="K13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>8</v>
+      </c>
+      <c r="J14" s="13">
+        <v>8</v>
+      </c>
+      <c r="K14" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="J15" s="12">
+        <v>9</v>
+      </c>
+      <c r="K15" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="33" x14ac:dyDescent="0.45">
+      <c r="G16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="7:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>5</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="7:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="G18" s="2">
+        <v>3</v>
+      </c>
+      <c r="H18" s="2">
+        <v>8</v>
+      </c>
+      <c r="J18" s="13">
+        <v>7</v>
+      </c>
+      <c r="K18" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="7:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>8</v>
+      </c>
+      <c r="J19" s="13">
+        <v>8</v>
+      </c>
+      <c r="K19" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="J20" s="13">
+        <v>9</v>
+      </c>
+      <c r="K20" s="13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>